<commit_message>
Updates on the obistat.owl, the Excel worksheet, and the PPT presentation after today's OBI conference call. Oliver He
</commit_message>
<xml_diff>
--- a/docs/presentations/OBI workshop May 2012 Ann Arbor/OBI Statistics/OBIstat source/OBIStat_new_terms_IDs-v2.xlsx
+++ b/docs/presentations/OBI workshop May 2012 Ann Arbor/OBI Statistics/OBIstat source/OBIStat_new_terms_IDs-v2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="559">
   <si>
     <t>Term ID</t>
   </si>
@@ -324,9 +324,6 @@
     <t>http://en.wikipedia.org/wiki/Cochran%E2%80%93Armitage_test_for_trend</t>
   </si>
   <si>
-    <t>collapsing</t>
-  </si>
-  <si>
     <t>a data transformation that combines categories or ranges of values to produce a smaller number of categories</t>
   </si>
   <si>
@@ -438,9 +435,6 @@
     <t>a variable specification that specifie a variable that may have a causal impact on both the independent variable and dependent variable; ignoring a confounding variable may bias empirical estimates of the causal effect of the independent variable.</t>
   </si>
   <si>
-    <t>confounders</t>
-  </si>
-  <si>
     <t>http://en.wikipedia.org/wiki/Mediation_%28statistics%29#Mediator_Variable</t>
   </si>
   <si>
@@ -453,9 +447,6 @@
     <t>dichotomous variable specification</t>
   </si>
   <si>
-    <t>a variable that has only two categories</t>
-  </si>
-  <si>
     <t xml:space="preserve">dichotomous variable </t>
   </si>
   <si>
@@ -633,15 +624,6 @@
     <t>sampling plan</t>
   </si>
   <si>
-    <t>a plan specification that provides a detailed outline of which measurements will be taken at what times, on which material, in what manner, and by whom.</t>
-  </si>
-  <si>
-    <t>plan specification</t>
-  </si>
-  <si>
-    <t>IAO_0000104</t>
-  </si>
-  <si>
     <t>http://www.itl.nist.gov/div898/handbook/ppc/section3/ppc33.htm</t>
   </si>
   <si>
@@ -739,9 +721,6 @@
   </si>
   <si>
     <t>random error</t>
-  </si>
-  <si>
-    <t>A component of experimental error that occurs due to natural variation in the process.</t>
   </si>
   <si>
     <t>range</t>
@@ -1733,6 +1712,24 @@
   </si>
   <si>
     <t>a data transformation that uses  measured variation in genes of known function to examine the causal effect of a modifiable exposure on disease in non-experimental studies.</t>
+  </si>
+  <si>
+    <t>a plan specification that provides a detailed outline of which measurements will be taken at what times, on which material samples, in what manner, and by whom.</t>
+  </si>
+  <si>
+    <t>a specification of a variable that has only two categories</t>
+  </si>
+  <si>
+    <t>confounder</t>
+  </si>
+  <si>
+    <t>A statistical error that occurs due to natural variation in the process.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>collapsing data transformation</t>
   </si>
 </sst>
 </file>
@@ -2132,8 +2129,8 @@
   <dimension ref="A1:L122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2187,24 +2184,24 @@
     </row>
     <row r="2" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="C2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>170</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7" t="s">
@@ -2214,19 +2211,19 @@
     </row>
     <row r="3" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -2241,24 +2238,24 @@
     </row>
     <row r="4" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
@@ -2268,22 +2265,22 @@
     </row>
     <row r="5" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
@@ -2295,19 +2292,19 @@
     </row>
     <row r="6" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -2324,40 +2321,40 @@
     </row>
     <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -2378,19 +2375,19 @@
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2405,16 +2402,16 @@
     </row>
     <row r="10" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2432,22 +2429,22 @@
     </row>
     <row r="11" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
@@ -2463,7 +2460,7 @@
     </row>
     <row r="12" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>66</v>
@@ -2492,7 +2489,7 @@
     </row>
     <row r="13" spans="1:11" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
@@ -2519,7 +2516,7 @@
     </row>
     <row r="14" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>99</v>
@@ -2548,22 +2545,22 @@
     </row>
     <row r="15" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7" t="s">
@@ -2579,19 +2576,19 @@
     </row>
     <row r="16" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -2604,7 +2601,7 @@
     </row>
     <row r="17" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>73</v>
@@ -2635,19 +2632,19 @@
     </row>
     <row r="18" spans="1:11" ht="90" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -2662,13 +2659,13 @@
     </row>
     <row r="19" spans="1:11" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>75</v>
@@ -2677,7 +2674,7 @@
         <v>76</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7" t="s">
@@ -2693,16 +2690,16 @@
     </row>
     <row r="20" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -2720,19 +2717,19 @@
     </row>
     <row r="21" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -2747,42 +2744,39 @@
     </row>
     <row r="22" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E22" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>140</v>
+        <v>555</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>46</v>
@@ -2791,7 +2785,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
@@ -2803,7 +2797,7 @@
     </row>
     <row r="24" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>81</v>
@@ -2832,19 +2826,19 @@
     </row>
     <row r="25" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" t="s">
         <v>136</v>
-      </c>
-      <c r="E25" t="s">
-        <v>137</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -2861,13 +2855,13 @@
     </row>
     <row r="26" spans="1:11" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>75</v>
@@ -2878,7 +2872,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1" t="s">
@@ -2890,19 +2884,19 @@
     </row>
     <row r="27" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -2917,22 +2911,19 @@
     </row>
     <row r="28" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>145</v>
+        <v>554</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E28" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
@@ -2940,7 +2931,7 @@
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>39</v>
@@ -2948,13 +2939,13 @@
     </row>
     <row r="29" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>46</v>
@@ -2963,7 +2954,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
@@ -2975,16 +2966,16 @@
     </row>
     <row r="30" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="1"/>
@@ -2997,21 +2988,21 @@
         <v>15</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="1"/>
@@ -3024,27 +3015,25 @@
         <v>15</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>137</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E32" s="7"/>
       <c r="F32" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
@@ -3060,24 +3049,24 @@
     </row>
     <row r="33" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
@@ -3089,7 +3078,7 @@
     </row>
     <row r="34" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>17</v>
@@ -3116,7 +3105,7 @@
     </row>
     <row r="35" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>20</v>
@@ -3145,24 +3134,24 @@
     </row>
     <row r="36" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="I36" s="8"/>
       <c r="J36" s="8" t="s">
@@ -3174,22 +3163,22 @@
     </row>
     <row r="37" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I37" s="8"/>
       <c r="J37" s="8" t="s">
@@ -3199,13 +3188,13 @@
     </row>
     <row r="38" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>46</v>
@@ -3214,7 +3203,7 @@
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="I38" s="8"/>
       <c r="J38" s="8" t="s">
@@ -3226,7 +3215,7 @@
     </row>
     <row r="39" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>24</v>
@@ -3235,7 +3224,7 @@
         <v>25</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
@@ -3253,24 +3242,24 @@
     </row>
     <row r="40" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>75</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1" t="s">
@@ -3282,7 +3271,7 @@
     </row>
     <row r="41" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>83</v>
@@ -3307,22 +3296,22 @@
     </row>
     <row r="42" spans="1:11" ht="90" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F42" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="G42" s="7"/>
       <c r="H42" s="7" t="s">
@@ -3336,24 +3325,24 @@
     </row>
     <row r="43" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="1" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1" t="s">
@@ -3365,19 +3354,19 @@
     </row>
     <row r="44" spans="1:11" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -3392,24 +3381,24 @@
     </row>
     <row r="45" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1" t="s">
@@ -3421,26 +3410,24 @@
     </row>
     <row r="46" spans="1:11" ht="131.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>137</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1" t="s">
@@ -3452,26 +3439,26 @@
     </row>
     <row r="47" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="7" t="s">
@@ -3483,13 +3470,13 @@
     </row>
     <row r="48" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>60</v>
@@ -3510,13 +3497,13 @@
     </row>
     <row r="49" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>75</v>
@@ -3527,7 +3514,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1" t="s">
@@ -3539,40 +3526,40 @@
     </row>
     <row r="50" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>75</v>
@@ -3583,7 +3570,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1" t="s">
@@ -3595,24 +3582,24 @@
     </row>
     <row r="52" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
       <c r="H52" s="8" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="I52" s="8"/>
       <c r="J52" s="11" t="s">
@@ -3622,13 +3609,13 @@
     </row>
     <row r="53" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C53" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>75</v>
@@ -3639,7 +3626,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1" t="s">
@@ -3649,26 +3636,26 @@
     </row>
     <row r="54" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1" t="s">
@@ -3680,13 +3667,13 @@
     </row>
     <row r="55" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="B55" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>75</v>
@@ -3697,7 +3684,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I55" s="1"/>
       <c r="J55" s="1" t="s">
@@ -3709,7 +3696,7 @@
     </row>
     <row r="56" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>40</v>
@@ -3736,26 +3723,26 @@
     </row>
     <row r="57" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="I57" s="1"/>
       <c r="J57" s="1" t="s">
@@ -3767,13 +3754,13 @@
     </row>
     <row r="58" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>75</v>
@@ -3784,7 +3771,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1" t="s">
@@ -3796,7 +3783,7 @@
     </row>
     <row r="59" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>50</v>
@@ -3827,13 +3814,13 @@
     </row>
     <row r="60" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>48</v>
@@ -3844,7 +3831,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1" t="s">
@@ -3854,29 +3841,29 @@
         <v>39</v>
       </c>
       <c r="L60" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1" t="s">
@@ -3886,13 +3873,13 @@
     </row>
     <row r="62" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>75</v>
@@ -3903,7 +3890,7 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1" t="s">
@@ -3913,26 +3900,26 @@
     </row>
     <row r="63" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="I63" s="7"/>
       <c r="J63" s="7" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="K63" s="7" t="s">
         <v>39</v>
@@ -3940,7 +3927,7 @@
     </row>
     <row r="64" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>69</v>
@@ -3969,24 +3956,24 @@
     </row>
     <row r="65" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
@@ -3996,16 +3983,16 @@
     </row>
     <row r="66" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E66" s="7"/>
       <c r="F66" s="7" t="s">
@@ -4021,7 +4008,7 @@
     </row>
     <row r="67" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>89</v>
@@ -4046,16 +4033,16 @@
     </row>
     <row r="68" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="7"/>
@@ -4068,24 +4055,24 @@
         <v>15</v>
       </c>
       <c r="K68" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="B69" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
@@ -4100,24 +4087,24 @@
     </row>
     <row r="70" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="B70" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
       <c r="H70" s="8" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="I70" s="8"/>
       <c r="J70" s="8" t="s">
@@ -4129,16 +4116,16 @@
     </row>
     <row r="71" spans="1:11" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
@@ -4154,7 +4141,7 @@
     </row>
     <row r="72" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>27</v>
@@ -4183,19 +4170,19 @@
     </row>
     <row r="73" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -4210,24 +4197,24 @@
     </row>
     <row r="74" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I74" s="1"/>
       <c r="J74" s="1" t="s">
@@ -4239,7 +4226,7 @@
     </row>
     <row r="75" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>55</v>
@@ -4268,13 +4255,13 @@
     </row>
     <row r="76" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B76" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C76" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>75</v>
@@ -4283,11 +4270,11 @@
         <v>76</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G76" s="8"/>
       <c r="H76" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I76" s="8"/>
       <c r="J76" s="8"/>
@@ -4295,19 +4282,19 @@
     </row>
     <row r="77" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -4322,16 +4309,16 @@
     </row>
     <row r="78" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -4344,12 +4331,12 @@
         <v>15</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>44</v>
@@ -4372,16 +4359,16 @@
     </row>
     <row r="80" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -4394,56 +4381,56 @@
         <v>15</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I81" s="1"/>
       <c r="J81" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I82" s="1"/>
       <c r="J82" s="1" t="s">
@@ -4455,16 +4442,16 @@
     </row>
     <row r="83" spans="1:11" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="7"/>
@@ -4477,24 +4464,24 @@
         <v>15</v>
       </c>
       <c r="K83" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -4509,7 +4496,7 @@
     </row>
     <row r="85" spans="1:11" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>91</v>
@@ -4536,22 +4523,22 @@
     </row>
     <row r="86" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1" t="s">
@@ -4565,26 +4552,26 @@
     </row>
     <row r="87" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>75</v>
       </c>
       <c r="E87" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="G87" s="1"/>
       <c r="H87" s="1" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="I87" s="1"/>
       <c r="J87" s="1" t="s">
@@ -4596,7 +4583,7 @@
     </row>
     <row r="88" spans="1:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>46</v>
@@ -4621,22 +4608,22 @@
     </row>
     <row r="89" spans="1:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="E89" s="8"/>
       <c r="F89" s="8"/>
       <c r="G89" s="8"/>
       <c r="H89" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I89" s="8"/>
       <c r="J89" s="8" t="s">
@@ -4646,51 +4633,51 @@
     </row>
     <row r="90" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>241</v>
+        <v>556</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="F90" s="8"/>
+        <v>307</v>
+      </c>
+      <c r="E90" s="7"/>
+      <c r="F90" s="8" t="s">
+        <v>557</v>
+      </c>
       <c r="G90" s="8"/>
       <c r="H90" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I90" s="8"/>
       <c r="J90" s="8" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="K90" s="8"/>
     </row>
     <row r="91" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D91" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F91" s="8"/>
       <c r="G91" s="8"/>
       <c r="H91" s="8" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="I91" s="8"/>
       <c r="J91" s="8" t="s">
@@ -4702,16 +4689,16 @@
     </row>
     <row r="92" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="E92" s="8"/>
       <c r="F92" s="8"/>
@@ -4727,19 +4714,19 @@
     </row>
     <row r="93" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
@@ -4754,19 +4741,19 @@
     </row>
     <row r="94" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
@@ -4781,13 +4768,13 @@
     </row>
     <row r="95" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>48</v>
@@ -4798,36 +4785,36 @@
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
       <c r="H95" s="7" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="I95" s="7"/>
       <c r="J95" s="7" t="s">
         <v>63</v>
       </c>
       <c r="K95" s="7" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="96" spans="1:11" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="I96" s="1"/>
       <c r="J96" s="1" t="s">
@@ -4837,19 +4824,19 @@
     </row>
     <row r="97" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
@@ -4864,19 +4851,19 @@
     </row>
     <row r="98" spans="1:11" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
@@ -4891,55 +4878,55 @@
     </row>
     <row r="99" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>205</v>
+        <v>553</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>206</v>
+        <v>327</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>207</v>
+        <v>328</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="G99" s="8"/>
       <c r="H99" s="8" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="I99" s="8"/>
       <c r="J99" s="8" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="K99" s="8"/>
     </row>
     <row r="100" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G100" s="7"/>
       <c r="H100" s="10" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="I100" s="7"/>
       <c r="J100" s="7" t="s">
@@ -4949,26 +4936,26 @@
     </row>
     <row r="101" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G101" s="7"/>
       <c r="H101" s="7" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="I101" s="7"/>
       <c r="J101" s="7" t="s">
@@ -4978,19 +4965,19 @@
     </row>
     <row r="102" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
@@ -5002,24 +4989,24 @@
         <v>15</v>
       </c>
       <c r="K102" s="7" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
@@ -5036,7 +5023,7 @@
     </row>
     <row r="104" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="B104" s="7" t="s">
         <v>96</v>
@@ -5063,13 +5050,13 @@
     </row>
     <row r="105" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="B105" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C105" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="D105" s="7" t="s">
         <v>75</v>
@@ -5078,11 +5065,11 @@
         <v>76</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G105" s="7"/>
       <c r="H105" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I105" s="7"/>
       <c r="J105" s="7" t="s">
@@ -5092,26 +5079,26 @@
     </row>
     <row r="106" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="G106" s="7"/>
       <c r="H106" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I106" s="7"/>
       <c r="J106" s="7" t="s">
@@ -5121,19 +5108,19 @@
     </row>
     <row r="107" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
@@ -5150,13 +5137,13 @@
     </row>
     <row r="108" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>75</v>
@@ -5165,11 +5152,11 @@
         <v>76</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G108" s="1"/>
       <c r="H108" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I108" s="1"/>
       <c r="J108" s="1" t="s">
@@ -5179,7 +5166,7 @@
     </row>
     <row r="109" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>32</v>
@@ -5208,7 +5195,7 @@
     </row>
     <row r="110" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>60</v>
@@ -5237,22 +5224,22 @@
     </row>
     <row r="111" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="G111" s="1"/>
       <c r="H111" s="1" t="s">
@@ -5266,22 +5253,22 @@
     </row>
     <row r="112" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="G112" s="7"/>
       <c r="H112" s="7" t="s">
@@ -5295,24 +5282,24 @@
     </row>
     <row r="113" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="E113" s="8"/>
       <c r="F113" s="8" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G113" s="8"/>
       <c r="H113" s="8" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="I113" s="8"/>
       <c r="J113" s="8" t="s">
@@ -5324,24 +5311,24 @@
     </row>
     <row r="114" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="E114" s="8"/>
       <c r="F114" s="8" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="G114" s="8"/>
       <c r="H114" s="8" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="I114" s="8"/>
       <c r="J114" s="8" t="s">
@@ -5353,7 +5340,7 @@
     </row>
     <row r="115" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>94</v>
@@ -5378,19 +5365,19 @@
     </row>
     <row r="116" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F116" s="7"/>
       <c r="G116" s="7"/>
@@ -5405,24 +5392,24 @@
     </row>
     <row r="117" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="B117" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C117" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C117" s="8" t="s">
+      <c r="D117" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D117" s="7" t="s">
+      <c r="E117" t="s">
         <v>136</v>
-      </c>
-      <c r="E117" t="s">
-        <v>137</v>
       </c>
       <c r="F117" s="8"/>
       <c r="G117" s="8"/>
       <c r="H117" s="8" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="I117" s="8"/>
       <c r="J117" s="8" t="s">
@@ -5432,7 +5419,7 @@
     </row>
     <row r="118" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>64</v>
@@ -5461,16 +5448,16 @@
     </row>
     <row r="119" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -5542,7 +5529,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -5560,7 +5547,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -5578,7 +5565,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -5596,7 +5583,7 @@
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>2</v>
@@ -5604,7 +5591,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -5614,7 +5601,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -5624,10 +5611,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -5636,10 +5623,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -5656,7 +5643,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5666,7 +5653,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -5676,7 +5663,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -5686,7 +5673,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -5696,7 +5683,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5706,7 +5693,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -5724,7 +5711,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -5734,7 +5721,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -5744,7 +5731,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -5762,7 +5749,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -5772,7 +5759,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -5782,7 +5769,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -5792,7 +5779,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -5810,7 +5797,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -5820,7 +5807,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -5830,7 +5817,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -5848,7 +5835,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -5858,7 +5845,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -5868,7 +5855,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -5878,11 +5865,11 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -5890,7 +5877,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -5900,7 +5887,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -5918,7 +5905,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -5928,7 +5915,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -5938,7 +5925,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -5948,7 +5935,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -5958,7 +5945,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -5968,7 +5955,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -5978,7 +5965,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -5996,7 +5983,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -6006,7 +5993,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -6016,7 +6003,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -6026,7 +6013,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -6054,7 +6041,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -6064,7 +6051,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -6074,7 +6061,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -6084,7 +6071,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>

</xml_diff>